<commit_message>
18.07.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Rajshahi_March'20 CO target vs Ach_BM _Dealer Channel (8.07.20).xlsx
+++ b/2020/Others/Rajshahi_March'20 CO target vs Ach_BM _Dealer Channel (8.07.20).xlsx
@@ -1,25 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RT BM\CO BM\2020\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7305" tabRatio="691" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7305" tabRatio="691" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet3" sheetId="80" state="hidden" r:id="rId1"/>
-    <sheet name="March'20 Incentive" sheetId="73" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="81" r:id="rId3"/>
+    <sheet name="Dealer wise summary _" sheetId="79" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="80" state="hidden" r:id="rId2"/>
+    <sheet name="March'20 Incentive" sheetId="73" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'March''20 Incentive'!$A$5:$L$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Dealer wise summary _'!$B$4:$H$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'March''20 Incentive'!$A$5:$P$21</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Dealer wise summary _'!$4:$4</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,12 +34,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="298">
   <si>
     <t>Retail ID</t>
   </si>
   <si>
     <t>Retail Name</t>
+  </si>
+  <si>
+    <t>Zone</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>SIS</t>
+  </si>
+  <si>
+    <t>Cap Imposed</t>
   </si>
   <si>
     <t>M/S Faiz Enterprise</t>
@@ -206,6 +225,9 @@
     <t>Hello Rajshahi</t>
   </si>
   <si>
+    <t>Rajshahi</t>
+  </si>
+  <si>
     <t>Haque Enterprise</t>
   </si>
   <si>
@@ -252,12 +274,6 @@
   </si>
   <si>
     <t>Rose Mobile Point</t>
-  </si>
-  <si>
-    <t>RET-08678</t>
-  </si>
-  <si>
-    <t>S.S Telecom</t>
   </si>
   <si>
     <t>RET-08755</t>
@@ -375,6 +391,9 @@
   </si>
   <si>
     <t>Dealer ID</t>
+  </si>
+  <si>
+    <t>RT Category</t>
   </si>
   <si>
     <t>A One Tel</t>
@@ -800,6 +819,21 @@
     <t>DEL-0177</t>
   </si>
   <si>
+    <t>Dealer Name</t>
+  </si>
+  <si>
+    <t>Prepared By -</t>
+  </si>
+  <si>
+    <t>Md. Taoshif Farik Huda</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Dealer wise summary</t>
+  </si>
+  <si>
     <t>RET-08762</t>
   </si>
   <si>
@@ -807,6 +841,9 @@
   </si>
   <si>
     <t>M/S. Karachi Store</t>
+  </si>
+  <si>
+    <t>Marketing</t>
   </si>
   <si>
     <t>DEL-0178</t>
@@ -834,6 +871,15 @@
   </si>
   <si>
     <t>Mugdho Corporation</t>
+  </si>
+  <si>
+    <t>SB Tel Amount</t>
+  </si>
+  <si>
+    <t>Industry Amount</t>
+  </si>
+  <si>
+    <t>Total Amount</t>
   </si>
   <si>
     <t>M/S. Sky Tel</t>
@@ -884,35 +930,18 @@
   <si>
     <t>Franchaise Outlet</t>
   </si>
-  <si>
-    <t>Retailer Signature</t>
-  </si>
-  <si>
-    <t>Target
- March'20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mugdho Corporation </t>
-  </si>
-  <si>
-    <t>Abdullah Plaza(1st Floor), Komola Super Market, Alaipur, Natore.</t>
-  </si>
-  <si>
-    <t>Date:</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
-    <numFmt numFmtId="167" formatCode="0.000%"/>
-    <numFmt numFmtId="168" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -958,56 +987,30 @@
       <name val="Calibri "/>
     </font>
     <font>
-      <sz val="25"/>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Malgun Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Malgun Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="1"/>
-      <name val="Malgun Gothic"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Malgun Gothic"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri "/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Calibri "/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Malgun Gothic"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Malgun Gothic"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1028,18 +1031,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1062,43 +1077,208 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1110,74 +1290,80 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="7" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="7" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1186,27 +1372,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1263,7 +1429,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Md. Taosif Farik Huda" refreshedDate="44020.68325613426" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="1308">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A5:J22" sheet="March'20 Incentive"/>
+    <worksheetSource ref="A5:O21" sheet="March'20 Incentive"/>
   </cacheSource>
   <cacheFields count="21">
     <cacheField name="Retail ID" numFmtId="0">
@@ -1530,25 +1696,25 @@
     <cacheField name="Cap Imposed" numFmtId="0">
       <sharedItems containsBlank="1"/>
     </cacheField>
-    <cacheField name="National total value target&#10; March'20" numFmtId="165">
+    <cacheField name="National total value target_x000a_ March'20" numFmtId="164">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="220000" maxValue="4000000"/>
     </cacheField>
-    <cacheField name="Achivement till 31 March'20" numFmtId="165">
+    <cacheField name="Achivement till 31 March'20" numFmtId="164">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="3517895"/>
     </cacheField>
     <cacheField name="Achievement %" numFmtId="9">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="2.0099999999999998"/>
     </cacheField>
-    <cacheField name="&gt;= 70% achv" numFmtId="167">
+    <cacheField name="&gt;= 70% achv" numFmtId="166">
       <sharedItems containsBlank="1"/>
     </cacheField>
-    <cacheField name="Secondary Sales Incentive Value" numFmtId="165">
+    <cacheField name="Secondary Sales Incentive Value" numFmtId="164">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="70400"/>
     </cacheField>
-    <cacheField name="SB Tel" numFmtId="165">
+    <cacheField name="SB Tel" numFmtId="164">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="2318515"/>
     </cacheField>
-    <cacheField name="Industry" numFmtId="165">
+    <cacheField name="Industry" numFmtId="164">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="1726660"/>
     </cacheField>
     <cacheField name="SB Tel2" numFmtId="9">
@@ -1563,10 +1729,10 @@
     <cacheField name="Industry3" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="36493"/>
     </cacheField>
-    <cacheField name="Model wise Incentive Value" numFmtId="165">
+    <cacheField name="Model wise Incentive Value" numFmtId="164">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="1770"/>
     </cacheField>
-    <cacheField name="Total Incentive" numFmtId="165">
+    <cacheField name="Total Incentive" numFmtId="164">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="70400"/>
     </cacheField>
   </cacheFields>
@@ -31668,7 +31834,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:C123" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="21">
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
@@ -31923,19 +32089,19 @@
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" numFmtId="165" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" numFmtId="165" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" numFmtId="164" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" numFmtId="164" outline="0" showAll="0" defaultSubtotal="0"/>
     <pivotField compact="0" numFmtId="9" outline="0" showAll="0" defaultSubtotal="0"/>
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" numFmtId="165" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" numFmtId="165" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" numFmtId="165" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" numFmtId="164" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" numFmtId="164" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" numFmtId="164" outline="0" showAll="0" defaultSubtotal="0"/>
     <pivotField compact="0" numFmtId="9" outline="0" showAll="0" defaultSubtotal="0"/>
     <pivotField compact="0" numFmtId="9" outline="0" showAll="0" defaultSubtotal="0"/>
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" numFmtId="165" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" compact="0" numFmtId="165" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" numFmtId="164" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" compact="0" numFmtId="164" outline="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="2">
     <field x="2"/>
@@ -32480,7 +32646,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -32515,7 +32681,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -32692,14 +32858,209 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:H15"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" style="9" customWidth="1"/>
+    <col min="4" max="5" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8">
+      <c r="B2" s="12" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="14.25" thickBot="1"/>
+    <row r="4" spans="2:8" ht="14.25" thickBot="1">
+      <c r="B4" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>261</v>
+      </c>
+      <c r="D4" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="46" t="s">
+        <v>279</v>
+      </c>
+      <c r="G4" s="46" t="s">
+        <v>280</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="15">
+      <c r="B5" s="48" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="42">
+        <v>1428</v>
+      </c>
+      <c r="G5" s="13">
+        <v>1143</v>
+      </c>
+      <c r="H5" s="49">
+        <f t="shared" ref="H5" si="0">F5+G5</f>
+        <v>2571</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B6" s="48" t="s">
+        <v>277</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>278</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="42">
+        <v>513</v>
+      </c>
+      <c r="G6" s="13">
+        <v>940</v>
+      </c>
+      <c r="H6" s="49">
+        <f t="shared" ref="H6:H7" si="1">F6+G6</f>
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B7" s="53" t="s">
+        <v>273</v>
+      </c>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="50">
+        <f>SUM(F5:F6)</f>
+        <v>1941</v>
+      </c>
+      <c r="G7" s="50">
+        <f>SUM(G5:G6)</f>
+        <v>2083</v>
+      </c>
+      <c r="H7" s="51">
+        <f t="shared" si="1"/>
+        <v>4024</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" s="45" customFormat="1" ht="15">
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+    </row>
+    <row r="9" spans="2:8" s="45" customFormat="1" ht="15">
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+    </row>
+    <row r="10" spans="2:8" s="45" customFormat="1" ht="15">
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+    </row>
+    <row r="11" spans="2:8" s="11" customFormat="1">
+      <c r="B11" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="38"/>
+    </row>
+    <row r="12" spans="2:8" s="11" customFormat="1">
+      <c r="B12" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="39"/>
+    </row>
+    <row r="13" spans="2:8" s="11" customFormat="1">
+      <c r="B13" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="39"/>
+    </row>
+    <row r="14" spans="2:8" s="11" customFormat="1">
+      <c r="B14" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="39"/>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="41"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="B4:H7">
+    <sortState ref="B5:H124">
+      <sortCondition ref="E4:E124"/>
+    </sortState>
+  </autoFilter>
+  <mergeCells count="1">
+    <mergeCell ref="B7:E7"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
+  <pageSetup scale="74" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C123"/>
   <sheetViews>
     <sheetView topLeftCell="A103" workbookViewId="0">
@@ -32714,1330 +33075,1330 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
-      <c r="A3" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>128</v>
+      <c r="A3" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>132</v>
       </c>
       <c r="C3" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C4" s="22">
+        <v>113</v>
+      </c>
+      <c r="C4" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="22">
+        <v>15</v>
+      </c>
+      <c r="C5" s="32">
         <v>2080</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="22">
+        <v>35</v>
+      </c>
+      <c r="C6" s="32">
         <v>6835</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="22">
+        <v>11</v>
+      </c>
+      <c r="C7" s="32">
         <v>6824</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="22">
+        <v>17</v>
+      </c>
+      <c r="C8" s="32">
         <v>3683</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
-      </c>
-      <c r="C9" s="22">
+        <v>112</v>
+      </c>
+      <c r="C9" s="32">
         <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="22">
+        <v>25</v>
+      </c>
+      <c r="C10" s="32">
         <v>10844</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="22">
+        <v>6</v>
+      </c>
+      <c r="C11" s="32">
         <v>21645</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C12" s="22">
+        <v>84</v>
+      </c>
+      <c r="C12" s="32">
         <v>12329</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="22">
+        <v>51</v>
+      </c>
+      <c r="C13" s="32">
         <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="B14" t="s">
-        <v>95</v>
-      </c>
-      <c r="C14" s="22">
+        <v>98</v>
+      </c>
+      <c r="C14" s="32">
         <v>9473</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="22">
+        <v>64</v>
+      </c>
+      <c r="C15" s="32">
         <v>225</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" s="22">
+        <v>74</v>
+      </c>
+      <c r="C16" s="32">
         <v>1820</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="22">
+        <v>43</v>
+      </c>
+      <c r="C17" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="22">
+        <v>62</v>
+      </c>
+      <c r="C18" s="32">
         <v>2866</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="22">
+        <v>36</v>
+      </c>
+      <c r="C19" s="32">
         <v>42156</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="22">
+        <v>42</v>
+      </c>
+      <c r="C20" s="32">
         <v>6168</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="22">
+        <v>21</v>
+      </c>
+      <c r="C21" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="22">
+        <v>38</v>
+      </c>
+      <c r="C22" s="32">
         <v>24681</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="22">
+        <v>13</v>
+      </c>
+      <c r="C23" s="32">
         <v>21589</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="22">
+        <v>34</v>
+      </c>
+      <c r="C24" s="32">
         <v>25809</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="22">
+        <v>37</v>
+      </c>
+      <c r="C25" s="32">
         <v>77149</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="22">
+        <v>7</v>
+      </c>
+      <c r="C26" s="32">
         <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B27" t="s">
-        <v>88</v>
-      </c>
-      <c r="C27" s="22">
+        <v>91</v>
+      </c>
+      <c r="C27" s="32">
         <v>12150</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="22">
+        <v>46</v>
+      </c>
+      <c r="C28" s="32">
         <v>76183</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" s="22">
+        <v>39</v>
+      </c>
+      <c r="C29" s="32">
         <v>16672</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="22">
+        <v>47</v>
+      </c>
+      <c r="C30" s="32">
         <v>4795</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
-      </c>
-      <c r="C31" s="22">
+        <v>24</v>
+      </c>
+      <c r="C31" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B32" t="s">
-        <v>240</v>
-      </c>
-      <c r="C32" s="22">
+        <v>244</v>
+      </c>
+      <c r="C32" s="32">
         <v>5101</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B33" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33" s="22">
+        <v>20</v>
+      </c>
+      <c r="C33" s="32">
         <v>14402</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B34" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" s="22">
+        <v>31</v>
+      </c>
+      <c r="C34" s="32">
         <v>891</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B35" t="s">
-        <v>54</v>
-      </c>
-      <c r="C35" s="22">
+        <v>58</v>
+      </c>
+      <c r="C35" s="32">
         <v>19484</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36" s="22">
+        <v>14</v>
+      </c>
+      <c r="C36" s="32">
         <v>32510</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="B37" t="s">
-        <v>99</v>
-      </c>
-      <c r="C37" s="22">
+        <v>102</v>
+      </c>
+      <c r="C37" s="32">
         <v>156151</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B38" t="s">
-        <v>108</v>
-      </c>
-      <c r="C38" s="22">
+        <v>111</v>
+      </c>
+      <c r="C38" s="32">
         <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B39" t="s">
-        <v>93</v>
-      </c>
-      <c r="C39" s="22">
+        <v>96</v>
+      </c>
+      <c r="C39" s="32">
         <v>902</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B40" t="s">
-        <v>56</v>
-      </c>
-      <c r="C40" s="22">
+        <v>60</v>
+      </c>
+      <c r="C40" s="32">
         <v>750</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B41" t="s">
-        <v>84</v>
-      </c>
-      <c r="C41" s="22">
+        <v>87</v>
+      </c>
+      <c r="C41" s="32">
         <v>22027</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B42" t="s">
-        <v>12</v>
-      </c>
-      <c r="C42" s="22">
+        <v>16</v>
+      </c>
+      <c r="C42" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="B43" t="s">
-        <v>105</v>
-      </c>
-      <c r="C43" s="22">
+        <v>108</v>
+      </c>
+      <c r="C43" s="32">
         <v>270</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B44" t="s">
-        <v>103</v>
-      </c>
-      <c r="C44" s="22">
+        <v>106</v>
+      </c>
+      <c r="C44" s="32">
         <v>40610</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
-      </c>
-      <c r="C45" s="22">
+        <v>86</v>
+      </c>
+      <c r="C45" s="32">
         <v>10275</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B46" t="s">
-        <v>87</v>
-      </c>
-      <c r="C46" s="22">
+        <v>90</v>
+      </c>
+      <c r="C46" s="32">
         <v>1203</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B47" t="s">
-        <v>23</v>
-      </c>
-      <c r="C47" s="22">
+        <v>27</v>
+      </c>
+      <c r="C47" s="32">
         <v>1156</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B48" t="s">
-        <v>15</v>
-      </c>
-      <c r="C48" s="22">
+        <v>19</v>
+      </c>
+      <c r="C48" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B49" t="s">
-        <v>44</v>
-      </c>
-      <c r="C49" s="22">
+        <v>48</v>
+      </c>
+      <c r="C49" s="32">
         <v>71944</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B50" t="s">
-        <v>49</v>
-      </c>
-      <c r="C50" s="22">
+        <v>53</v>
+      </c>
+      <c r="C50" s="32">
         <v>18886</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B51" t="s">
-        <v>65</v>
-      </c>
-      <c r="C51" s="22">
+        <v>70</v>
+      </c>
+      <c r="C51" s="32">
         <v>16246</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="B52" t="s">
-        <v>40</v>
-      </c>
-      <c r="C52" s="22">
+        <v>44</v>
+      </c>
+      <c r="C52" s="32">
         <v>26062</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="B53" t="s">
-        <v>102</v>
-      </c>
-      <c r="C53" s="22">
+        <v>105</v>
+      </c>
+      <c r="C53" s="32">
         <v>41820</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B54" t="s">
-        <v>14</v>
-      </c>
-      <c r="C54" s="22">
+        <v>18</v>
+      </c>
+      <c r="C54" s="32">
         <v>6150</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B55" t="s">
-        <v>272</v>
-      </c>
-      <c r="C55" s="22">
+        <v>285</v>
+      </c>
+      <c r="C55" s="32">
         <v>4147</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B56" t="s">
-        <v>60</v>
-      </c>
-      <c r="C56" s="22">
+        <v>65</v>
+      </c>
+      <c r="C56" s="32">
         <v>5946</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B57" t="s">
-        <v>90</v>
-      </c>
-      <c r="C57" s="22">
+        <v>93</v>
+      </c>
+      <c r="C57" s="32">
         <v>1753</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B58" t="s">
-        <v>24</v>
-      </c>
-      <c r="C58" s="22">
+        <v>28</v>
+      </c>
+      <c r="C58" s="32">
         <v>5508</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="B59" t="s">
-        <v>37</v>
-      </c>
-      <c r="C59" s="22">
+        <v>41</v>
+      </c>
+      <c r="C59" s="32">
         <v>26831</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B60" t="s">
-        <v>45</v>
-      </c>
-      <c r="C60" s="22">
+        <v>49</v>
+      </c>
+      <c r="C60" s="32">
         <v>7892</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B61" t="s">
-        <v>53</v>
-      </c>
-      <c r="C61" s="22">
+        <v>57</v>
+      </c>
+      <c r="C61" s="32">
         <v>35742</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B62" t="s">
-        <v>51</v>
-      </c>
-      <c r="C62" s="22">
+        <v>55</v>
+      </c>
+      <c r="C62" s="32">
         <v>18582</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B63" t="s">
-        <v>96</v>
-      </c>
-      <c r="C63" s="22">
+        <v>99</v>
+      </c>
+      <c r="C63" s="32">
         <v>36497</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B64" t="s">
-        <v>46</v>
-      </c>
-      <c r="C64" s="22">
+        <v>50</v>
+      </c>
+      <c r="C64" s="32">
         <v>2941</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B65" t="s">
-        <v>55</v>
-      </c>
-      <c r="C65" s="22">
+        <v>59</v>
+      </c>
+      <c r="C65" s="32">
         <v>9871</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B66" t="s">
-        <v>106</v>
-      </c>
-      <c r="C66" s="22">
+        <v>109</v>
+      </c>
+      <c r="C66" s="32">
         <v>16819</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B67" t="s">
-        <v>86</v>
-      </c>
-      <c r="C67" s="22">
+        <v>89</v>
+      </c>
+      <c r="C67" s="32">
         <v>50033</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="B68" t="s">
-        <v>101</v>
-      </c>
-      <c r="C68" s="22">
+        <v>104</v>
+      </c>
+      <c r="C68" s="32">
         <v>120237</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B69" t="s">
-        <v>25</v>
-      </c>
-      <c r="C69" s="22">
+        <v>29</v>
+      </c>
+      <c r="C69" s="32">
         <v>11376</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="B70" t="s">
-        <v>6</v>
-      </c>
-      <c r="C70" s="22">
+        <v>10</v>
+      </c>
+      <c r="C70" s="32">
         <v>22480</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B71" t="s">
-        <v>89</v>
-      </c>
-      <c r="C71" s="22">
+        <v>92</v>
+      </c>
+      <c r="C71" s="32">
         <v>44518</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="B72" t="s">
-        <v>97</v>
-      </c>
-      <c r="C72" s="22">
+        <v>100</v>
+      </c>
+      <c r="C72" s="32">
         <v>120423</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B73" t="s">
-        <v>92</v>
-      </c>
-      <c r="C73" s="22">
+        <v>95</v>
+      </c>
+      <c r="C73" s="32">
         <v>31583</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="B74" t="s">
-        <v>100</v>
-      </c>
-      <c r="C74" s="22">
+        <v>103</v>
+      </c>
+      <c r="C74" s="32">
         <v>29521</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B75" t="s">
-        <v>104</v>
-      </c>
-      <c r="C75" s="22">
+        <v>107</v>
+      </c>
+      <c r="C75" s="32">
         <v>4935</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B76" t="s">
-        <v>111</v>
-      </c>
-      <c r="C76" s="22">
+        <v>114</v>
+      </c>
+      <c r="C76" s="32">
         <v>880</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B77" t="s">
-        <v>107</v>
-      </c>
-      <c r="C77" s="22">
+        <v>110</v>
+      </c>
+      <c r="C77" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="B78" t="s">
-        <v>284</v>
-      </c>
-      <c r="C78" s="22">
+        <v>297</v>
+      </c>
+      <c r="C78" s="32">
         <v>376329</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="B79" t="s">
-        <v>36</v>
-      </c>
-      <c r="C79" s="22">
+        <v>40</v>
+      </c>
+      <c r="C79" s="32">
         <v>6654</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="B80" t="s">
-        <v>94</v>
-      </c>
-      <c r="C80" s="22">
+        <v>97</v>
+      </c>
+      <c r="C80" s="32">
         <v>11477</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B81" t="s">
-        <v>91</v>
-      </c>
-      <c r="C81" s="22">
+        <v>94</v>
+      </c>
+      <c r="C81" s="32">
         <v>360</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B82" t="s">
-        <v>66</v>
-      </c>
-      <c r="C82" s="22">
+        <v>71</v>
+      </c>
+      <c r="C82" s="32">
         <v>8782</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B83" t="s">
-        <v>52</v>
-      </c>
-      <c r="C83" s="22">
+        <v>56</v>
+      </c>
+      <c r="C83" s="32">
         <v>41050</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="B84" t="s">
-        <v>239</v>
-      </c>
-      <c r="C84" s="22">
+        <v>243</v>
+      </c>
+      <c r="C84" s="32">
         <v>4052</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B85" t="s">
-        <v>82</v>
-      </c>
-      <c r="C85" s="22">
+        <v>85</v>
+      </c>
+      <c r="C85" s="32">
         <v>22573</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="B86" t="s">
-        <v>98</v>
-      </c>
-      <c r="C86" s="22">
+        <v>101</v>
+      </c>
+      <c r="C86" s="32">
         <v>18447</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B87" t="s">
-        <v>8</v>
-      </c>
-      <c r="C87" s="22">
+        <v>12</v>
+      </c>
+      <c r="C87" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B88" t="s">
-        <v>50</v>
-      </c>
-      <c r="C88" s="22">
+        <v>54</v>
+      </c>
+      <c r="C88" s="32">
         <v>40065</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B89" t="s">
-        <v>26</v>
-      </c>
-      <c r="C89" s="22">
+        <v>30</v>
+      </c>
+      <c r="C89" s="32">
         <v>1344</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B90" t="s">
-        <v>5</v>
-      </c>
-      <c r="C90" s="22">
+        <v>9</v>
+      </c>
+      <c r="C90" s="32">
         <v>8537</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B91" t="s">
-        <v>85</v>
-      </c>
-      <c r="C91" s="22">
+        <v>88</v>
+      </c>
+      <c r="C91" s="32">
         <v>8377</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B92" t="s">
-        <v>18</v>
-      </c>
-      <c r="C92" s="22">
+        <v>22</v>
+      </c>
+      <c r="C92" s="32">
         <v>8600</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B93" t="s">
-        <v>113</v>
-      </c>
-      <c r="C93" s="22">
+        <v>116</v>
+      </c>
+      <c r="C93" s="32">
         <v>7594</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B94" t="s">
-        <v>4</v>
-      </c>
-      <c r="C94" s="22">
+        <v>8</v>
+      </c>
+      <c r="C94" s="32">
         <v>5093</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B95" t="s">
-        <v>19</v>
-      </c>
-      <c r="C95" s="22">
+        <v>23</v>
+      </c>
+      <c r="C95" s="32">
         <v>1920</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B96" t="s">
-        <v>121</v>
-      </c>
-      <c r="C96" s="22">
+        <v>125</v>
+      </c>
+      <c r="C96" s="32">
         <v>14488</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B97" t="s">
-        <v>114</v>
-      </c>
-      <c r="C97" s="22">
+        <v>117</v>
+      </c>
+      <c r="C97" s="32">
         <v>9518</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="B98" t="s">
-        <v>116</v>
-      </c>
-      <c r="C98" s="22">
+        <v>120</v>
+      </c>
+      <c r="C98" s="32">
         <v>21752</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="B99" t="s">
-        <v>119</v>
-      </c>
-      <c r="C99" s="22">
+        <v>123</v>
+      </c>
+      <c r="C99" s="32">
         <v>4127</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B100" t="s">
-        <v>120</v>
-      </c>
-      <c r="C100" s="22">
+        <v>124</v>
+      </c>
+      <c r="C100" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B101" t="s">
-        <v>118</v>
-      </c>
-      <c r="C101" s="22">
+        <v>122</v>
+      </c>
+      <c r="C101" s="32">
         <v>3239</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B102" t="s">
-        <v>122</v>
-      </c>
-      <c r="C102" s="22">
+        <v>126</v>
+      </c>
+      <c r="C102" s="32">
         <v>29530</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B103" t="s">
-        <v>125</v>
-      </c>
-      <c r="C103" s="22">
+        <v>129</v>
+      </c>
+      <c r="C103" s="32">
         <v>108911</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B104" t="s">
-        <v>117</v>
-      </c>
-      <c r="C104" s="22">
+        <v>121</v>
+      </c>
+      <c r="C104" s="32">
         <v>179129</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B105" t="s">
-        <v>123</v>
-      </c>
-      <c r="C105" s="22">
+        <v>127</v>
+      </c>
+      <c r="C105" s="32">
         <v>1103</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="B106" t="s">
-        <v>57</v>
-      </c>
-      <c r="C106" s="22">
+        <v>61</v>
+      </c>
+      <c r="C106" s="32">
         <v>23175</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B107" t="s">
-        <v>124</v>
-      </c>
-      <c r="C107" s="22">
+        <v>128</v>
+      </c>
+      <c r="C107" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B108" t="s">
-        <v>274</v>
-      </c>
-      <c r="C108" s="22">
+        <v>287</v>
+      </c>
+      <c r="C108" s="32">
         <v>5200</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B109" t="s">
-        <v>127</v>
-      </c>
-      <c r="C109" s="22">
+        <v>131</v>
+      </c>
+      <c r="C109" s="32">
         <v>76054</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B110" t="s">
-        <v>126</v>
-      </c>
-      <c r="C110" s="22">
+        <v>130</v>
+      </c>
+      <c r="C110" s="32">
         <v>3818</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="B111" t="s">
-        <v>133</v>
-      </c>
-      <c r="C111" s="22">
+        <v>137</v>
+      </c>
+      <c r="C111" s="32">
         <v>24854</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="B112" t="s">
-        <v>265</v>
-      </c>
-      <c r="C112" s="22">
+        <v>275</v>
+      </c>
+      <c r="C112" s="32">
         <v>4666</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="B113" t="s">
-        <v>246</v>
-      </c>
-      <c r="C113" s="22">
+        <v>250</v>
+      </c>
+      <c r="C113" s="32">
         <v>1175</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B114" t="s">
-        <v>253</v>
-      </c>
-      <c r="C114" s="22">
+        <v>257</v>
+      </c>
+      <c r="C114" s="32">
         <v>13484</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="B115" t="s">
-        <v>259</v>
-      </c>
-      <c r="C115" s="22">
+        <v>268</v>
+      </c>
+      <c r="C115" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="B116" t="s">
-        <v>255</v>
-      </c>
-      <c r="C116" s="22">
+        <v>259</v>
+      </c>
+      <c r="C116" s="32">
         <v>5028</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="B117" t="s">
-        <v>261</v>
-      </c>
-      <c r="C117" s="22">
+        <v>271</v>
+      </c>
+      <c r="C117" s="32">
         <v>36672</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="B118" t="s">
-        <v>268</v>
-      </c>
-      <c r="C118" s="22">
+        <v>278</v>
+      </c>
+      <c r="C118" s="32">
         <v>1543</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>275</v>
+        <v>288</v>
       </c>
       <c r="B119" t="s">
-        <v>269</v>
-      </c>
-      <c r="C119" s="22">
+        <v>282</v>
+      </c>
+      <c r="C119" s="32">
         <v>7664</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>273</v>
+        <v>286</v>
       </c>
       <c r="B120" t="s">
-        <v>262</v>
-      </c>
-      <c r="C120" s="22">
+        <v>272</v>
+      </c>
+      <c r="C120" s="32">
         <v>2916</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>280</v>
+        <v>293</v>
       </c>
       <c r="B121" t="s">
-        <v>281</v>
-      </c>
-      <c r="C121" s="22">
+        <v>294</v>
+      </c>
+      <c r="C121" s="32">
         <v>4981</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>282</v>
+        <v>295</v>
       </c>
       <c r="B122" t="s">
-        <v>283</v>
-      </c>
-      <c r="C122" s="22">
+        <v>296</v>
+      </c>
+      <c r="C122" s="32">
         <v>880</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>263</v>
-      </c>
-      <c r="C123" s="22">
+        <v>273</v>
+      </c>
+      <c r="C123" s="32">
         <v>2636957</v>
       </c>
     </row>
@@ -34046,930 +34407,811 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A2:M22"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:Q21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="5" topLeftCell="I6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5:K22"/>
+      <selection pane="bottomRight" activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" style="14" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="23"/>
+    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="23" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13">
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
+    <row r="2" spans="1:17">
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
     </row>
-    <row r="3" spans="1:13">
-      <c r="E3" s="7"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
+    <row r="3" spans="1:17">
+      <c r="J3" s="8"/>
+      <c r="O3" s="15"/>
     </row>
-    <row r="4" spans="1:13">
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
+    <row r="4" spans="1:17">
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
     </row>
-    <row r="5" spans="1:13" ht="40.5">
-      <c r="A5" s="16" t="s">
+    <row r="5" spans="1:17" ht="38.25">
+      <c r="A5" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>276</v>
-      </c>
-      <c r="E5" s="11" t="s">
+      <c r="C5" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="29" t="s">
+        <v>289</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>290</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>292</v>
+      </c>
+      <c r="M5" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="N5" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="O5" s="30" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="24">
+        <v>450000</v>
+      </c>
+      <c r="J6" s="2">
+        <v>417780</v>
+      </c>
+      <c r="K6" s="35">
+        <v>0.93</v>
+      </c>
+      <c r="L6" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="M6" s="14">
+        <v>2511</v>
+      </c>
+      <c r="N6" s="5">
+        <v>60</v>
+      </c>
+      <c r="O6" s="31">
+        <v>2571</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="24">
+        <v>350000</v>
+      </c>
+      <c r="J7" s="2">
+        <v>66235</v>
+      </c>
+      <c r="K7" s="35">
+        <v>0.19</v>
+      </c>
+      <c r="L7" s="34"/>
+      <c r="M7" s="14">
+        <v>0</v>
+      </c>
+      <c r="N7" s="5">
+        <v>0</v>
+      </c>
+      <c r="O7" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="24">
+        <v>400000</v>
+      </c>
+      <c r="J8" s="2">
+        <v>227655</v>
+      </c>
+      <c r="K8" s="35">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="L8" s="34"/>
+      <c r="M8" s="14">
+        <v>0</v>
+      </c>
+      <c r="N8" s="5">
+        <v>0</v>
+      </c>
+      <c r="O8" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="24">
+        <v>400000</v>
+      </c>
+      <c r="J9" s="2">
+        <v>216755</v>
+      </c>
+      <c r="K9" s="35">
+        <v>0.54</v>
+      </c>
+      <c r="L9" s="34"/>
+      <c r="M9" s="14">
+        <v>0</v>
+      </c>
+      <c r="N9" s="5">
+        <v>0</v>
+      </c>
+      <c r="O9" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="24">
+        <v>350000</v>
+      </c>
+      <c r="J10" s="2">
+        <v>166610</v>
+      </c>
+      <c r="K10" s="35">
+        <v>0.48</v>
+      </c>
+      <c r="L10" s="34"/>
+      <c r="M10" s="14">
+        <v>0</v>
+      </c>
+      <c r="N10" s="5">
+        <v>0</v>
+      </c>
+      <c r="O10" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="24">
+        <v>300000</v>
+      </c>
+      <c r="J11" s="2">
+        <v>70180</v>
+      </c>
+      <c r="K11" s="35">
+        <v>0.23</v>
+      </c>
+      <c r="L11" s="34"/>
+      <c r="M11" s="14">
+        <v>0</v>
+      </c>
+      <c r="N11" s="5">
+        <v>0</v>
+      </c>
+      <c r="O11" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="24">
+        <v>220000</v>
+      </c>
+      <c r="J12" s="2">
+        <v>71835</v>
+      </c>
+      <c r="K12" s="35">
+        <v>0.33</v>
+      </c>
+      <c r="L12" s="34"/>
+      <c r="M12" s="14">
+        <v>0</v>
+      </c>
+      <c r="N12" s="5">
+        <v>0</v>
+      </c>
+      <c r="O12" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="24">
+        <v>220000</v>
+      </c>
+      <c r="J13" s="2">
+        <v>150940</v>
+      </c>
+      <c r="K13" s="35">
+        <v>0.69</v>
+      </c>
+      <c r="L13" s="34"/>
+      <c r="M13" s="14">
+        <v>0</v>
+      </c>
+      <c r="N13" s="5">
+        <v>0</v>
+      </c>
+      <c r="O13" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="24">
+        <v>325000</v>
+      </c>
+      <c r="J14" s="2">
+        <v>148215</v>
+      </c>
+      <c r="K14" s="35">
+        <v>0.46</v>
+      </c>
+      <c r="L14" s="34"/>
+      <c r="M14" s="14">
+        <v>0</v>
+      </c>
+      <c r="N14" s="5">
+        <v>0</v>
+      </c>
+      <c r="O14" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="24">
+        <v>300000</v>
+      </c>
+      <c r="J15" s="2">
+        <v>115875</v>
+      </c>
+      <c r="K15" s="35">
+        <v>0.39</v>
+      </c>
+      <c r="L15" s="34"/>
+      <c r="M15" s="14">
+        <v>0</v>
+      </c>
+      <c r="N15" s="5">
+        <v>0</v>
+      </c>
+      <c r="O15" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>279</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="J5" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="K5" s="26" t="s">
-        <v>285</v>
+      <c r="D16" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="24">
+        <v>1300000</v>
+      </c>
+      <c r="J16" s="2">
+        <v>678155</v>
+      </c>
+      <c r="K16" s="35">
+        <v>0.52</v>
+      </c>
+      <c r="L16" s="34"/>
+      <c r="M16" s="14">
+        <v>0</v>
+      </c>
+      <c r="N16" s="5">
+        <v>0</v>
+      </c>
+      <c r="O16" s="31">
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1">
-      <c r="A6" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="15">
-        <v>625000</v>
-      </c>
-      <c r="E6" s="1">
-        <v>260760</v>
-      </c>
-      <c r="F6" s="25">
-        <v>0.42</v>
-      </c>
-      <c r="G6" s="24"/>
-      <c r="H6" s="8">
+    <row r="17" spans="1:15">
+      <c r="A17" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="24">
+        <v>1000000</v>
+      </c>
+      <c r="J17" s="2">
+        <v>623245</v>
+      </c>
+      <c r="K17" s="35">
+        <v>0.62</v>
+      </c>
+      <c r="L17" s="34"/>
+      <c r="M17" s="14">
         <v>0</v>
       </c>
-      <c r="I6" s="4">
+      <c r="N17" s="5">
         <v>0</v>
       </c>
-      <c r="J6" s="21">
+      <c r="O17" s="31">
         <v>0</v>
       </c>
-      <c r="K6" s="21"/>
     </row>
-    <row r="7" spans="1:13" hidden="1">
-      <c r="A7" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="15">
-        <v>450000</v>
-      </c>
-      <c r="E7" s="1">
-        <v>417780</v>
-      </c>
-      <c r="F7" s="25">
-        <v>0.93</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="H7" s="8">
-        <v>2511</v>
-      </c>
-      <c r="I7" s="4">
+    <row r="18" spans="1:15">
+      <c r="A18" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="24">
+        <v>900000</v>
+      </c>
+      <c r="J18" s="2">
+        <v>556360</v>
+      </c>
+      <c r="K18" s="35">
+        <v>0.62</v>
+      </c>
+      <c r="L18" s="34"/>
+      <c r="M18" s="14">
         <v>0</v>
       </c>
-      <c r="J7" s="21">
-        <v>2511</v>
-      </c>
-      <c r="K7" s="21"/>
+      <c r="N18" s="5">
+        <v>0</v>
+      </c>
+      <c r="O18" s="31">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:13" hidden="1">
-      <c r="A8" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="15">
+    <row r="19" spans="1:15">
+      <c r="A19" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="24">
+        <v>800000</v>
+      </c>
+      <c r="J19" s="2">
+        <v>438740</v>
+      </c>
+      <c r="K19" s="35">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L19" s="34"/>
+      <c r="M19" s="14">
+        <v>0</v>
+      </c>
+      <c r="N19" s="5">
+        <v>0</v>
+      </c>
+      <c r="O19" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="24">
+        <v>381157</v>
+      </c>
+      <c r="J20" s="2">
+        <v>251605</v>
+      </c>
+      <c r="K20" s="35">
+        <v>0.66</v>
+      </c>
+      <c r="L20" s="34"/>
+      <c r="M20" s="14">
+        <v>0</v>
+      </c>
+      <c r="N20" s="5">
+        <v>0</v>
+      </c>
+      <c r="O20" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="24">
         <v>350000</v>
       </c>
-      <c r="E8" s="1">
-        <v>66235</v>
-      </c>
-      <c r="F8" s="25">
-        <v>0.19</v>
-      </c>
-      <c r="G8" s="24"/>
-      <c r="H8" s="8">
+      <c r="J21" s="2">
+        <v>291550</v>
+      </c>
+      <c r="K21" s="35">
+        <v>0.83</v>
+      </c>
+      <c r="L21" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="M21" s="14">
+        <v>1453</v>
+      </c>
+      <c r="N21" s="5">
         <v>0</v>
       </c>
-      <c r="I8" s="4">
-        <v>135</v>
-      </c>
-      <c r="J8" s="21">
-        <v>135</v>
-      </c>
-      <c r="K8" s="21"/>
-    </row>
-    <row r="9" spans="1:13" hidden="1">
-      <c r="A9" s="6" t="s">
-        <v>257</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="15">
-        <v>400000</v>
-      </c>
-      <c r="E9" s="1">
-        <v>227655</v>
-      </c>
-      <c r="F9" s="25">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="G9" s="24"/>
-      <c r="H9" s="8">
-        <v>0</v>
-      </c>
-      <c r="I9" s="4">
-        <v>0</v>
-      </c>
-      <c r="J9" s="21">
-        <v>0</v>
-      </c>
-      <c r="K9" s="21"/>
-    </row>
-    <row r="10" spans="1:13" hidden="1">
-      <c r="A10" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="15">
-        <v>400000</v>
-      </c>
-      <c r="E10" s="1">
-        <v>216755</v>
-      </c>
-      <c r="F10" s="25">
-        <v>0.54</v>
-      </c>
-      <c r="G10" s="24"/>
-      <c r="H10" s="8">
-        <v>0</v>
-      </c>
-      <c r="I10" s="4">
-        <v>220</v>
-      </c>
-      <c r="J10" s="21">
-        <v>220</v>
-      </c>
-      <c r="K10" s="21"/>
-    </row>
-    <row r="11" spans="1:13" hidden="1">
-      <c r="A11" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="15">
-        <v>350000</v>
-      </c>
-      <c r="E11" s="1">
-        <v>166610</v>
-      </c>
-      <c r="F11" s="25">
-        <v>0.48</v>
-      </c>
-      <c r="G11" s="24"/>
-      <c r="H11" s="8">
-        <v>0</v>
-      </c>
-      <c r="I11" s="4">
-        <v>0</v>
-      </c>
-      <c r="J11" s="21">
-        <v>0</v>
-      </c>
-      <c r="K11" s="21"/>
-    </row>
-    <row r="12" spans="1:13" hidden="1">
-      <c r="A12" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="15">
-        <v>300000</v>
-      </c>
-      <c r="E12" s="1">
-        <v>70180</v>
-      </c>
-      <c r="F12" s="25">
-        <v>0.23</v>
-      </c>
-      <c r="G12" s="24"/>
-      <c r="H12" s="8">
-        <v>0</v>
-      </c>
-      <c r="I12" s="4">
-        <v>0</v>
-      </c>
-      <c r="J12" s="21">
-        <v>0</v>
-      </c>
-      <c r="K12" s="21"/>
-    </row>
-    <row r="13" spans="1:13" hidden="1">
-      <c r="A13" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="15">
-        <v>220000</v>
-      </c>
-      <c r="E13" s="1">
-        <v>71835</v>
-      </c>
-      <c r="F13" s="25">
-        <v>0.33</v>
-      </c>
-      <c r="G13" s="24"/>
-      <c r="H13" s="8">
-        <v>0</v>
-      </c>
-      <c r="I13" s="4">
-        <v>0</v>
-      </c>
-      <c r="J13" s="21">
-        <v>0</v>
-      </c>
-      <c r="K13" s="21"/>
-    </row>
-    <row r="14" spans="1:13" hidden="1">
-      <c r="A14" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="15">
-        <v>220000</v>
-      </c>
-      <c r="E14" s="1">
-        <v>150940</v>
-      </c>
-      <c r="F14" s="25">
-        <v>0.69</v>
-      </c>
-      <c r="G14" s="24"/>
-      <c r="H14" s="8">
-        <v>0</v>
-      </c>
-      <c r="I14" s="4">
-        <v>0</v>
-      </c>
-      <c r="J14" s="21">
-        <v>0</v>
-      </c>
-      <c r="K14" s="21"/>
-    </row>
-    <row r="15" spans="1:13" hidden="1">
-      <c r="A15" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="15">
-        <v>325000</v>
-      </c>
-      <c r="E15" s="1">
-        <v>148215</v>
-      </c>
-      <c r="F15" s="25">
-        <v>0.46</v>
-      </c>
-      <c r="G15" s="24"/>
-      <c r="H15" s="8">
-        <v>0</v>
-      </c>
-      <c r="I15" s="4">
-        <v>0</v>
-      </c>
-      <c r="J15" s="21">
-        <v>0</v>
-      </c>
-      <c r="K15" s="21"/>
-    </row>
-    <row r="16" spans="1:13" hidden="1">
-      <c r="A16" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="15">
-        <v>300000</v>
-      </c>
-      <c r="E16" s="1">
-        <v>115875</v>
-      </c>
-      <c r="F16" s="25">
-        <v>0.39</v>
-      </c>
-      <c r="G16" s="24"/>
-      <c r="H16" s="8">
-        <v>0</v>
-      </c>
-      <c r="I16" s="4">
-        <v>0</v>
-      </c>
-      <c r="J16" s="21">
-        <v>0</v>
-      </c>
-      <c r="K16" s="21"/>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="D17" s="15">
-        <v>1300000</v>
-      </c>
-      <c r="E17" s="1">
-        <v>678155</v>
-      </c>
-      <c r="F17" s="25">
-        <v>0.52</v>
-      </c>
-      <c r="G17" s="24"/>
-      <c r="H17" s="8">
-        <v>0</v>
-      </c>
-      <c r="I17" s="4">
-        <v>0</v>
-      </c>
-      <c r="J17" s="21">
-        <v>0</v>
-      </c>
-      <c r="K17" s="21"/>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="D18" s="15">
-        <v>1000000</v>
-      </c>
-      <c r="E18" s="1">
-        <v>623245</v>
-      </c>
-      <c r="F18" s="25">
-        <v>0.62</v>
-      </c>
-      <c r="G18" s="24"/>
-      <c r="H18" s="8">
-        <v>0</v>
-      </c>
-      <c r="I18" s="4">
-        <v>0</v>
-      </c>
-      <c r="J18" s="21">
-        <v>0</v>
-      </c>
-      <c r="K18" s="21"/>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="D19" s="15">
-        <v>900000</v>
-      </c>
-      <c r="E19" s="1">
-        <v>556360</v>
-      </c>
-      <c r="F19" s="25">
-        <v>0.62</v>
-      </c>
-      <c r="G19" s="24"/>
-      <c r="H19" s="8">
-        <v>0</v>
-      </c>
-      <c r="I19" s="4">
-        <v>0</v>
-      </c>
-      <c r="J19" s="21">
-        <v>0</v>
-      </c>
-      <c r="K19" s="21"/>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="D20" s="15">
-        <v>800000</v>
-      </c>
-      <c r="E20" s="1">
-        <v>438740</v>
-      </c>
-      <c r="F20" s="25">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="G20" s="24"/>
-      <c r="H20" s="8">
-        <v>0</v>
-      </c>
-      <c r="I20" s="4">
-        <v>90</v>
-      </c>
-      <c r="J20" s="21">
-        <v>90</v>
-      </c>
-      <c r="K20" s="21"/>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="D21" s="15">
-        <v>381157</v>
-      </c>
-      <c r="E21" s="1">
-        <v>251605</v>
-      </c>
-      <c r="F21" s="25">
-        <v>0.66</v>
-      </c>
-      <c r="G21" s="24"/>
-      <c r="H21" s="8">
-        <v>0</v>
-      </c>
-      <c r="I21" s="4">
-        <v>0</v>
-      </c>
-      <c r="J21" s="21">
-        <v>0</v>
-      </c>
-      <c r="K21" s="21"/>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="D22" s="15">
-        <v>350000</v>
-      </c>
-      <c r="E22" s="1">
-        <v>291550</v>
-      </c>
-      <c r="F22" s="25">
-        <v>0.83</v>
-      </c>
-      <c r="G22" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="H22" s="8">
+      <c r="O21" s="31">
         <v>1453</v>
       </c>
-      <c r="I22" s="4">
-        <v>0</v>
-      </c>
-      <c r="J22" s="21">
-        <v>1453</v>
-      </c>
-      <c r="K22" s="21"/>
     </row>
   </sheetData>
-  <autoFilter ref="A5:L22">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Mugdho Corporation"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A5:P21"/>
   <conditionalFormatting sqref="A5">
-    <cfRule type="duplicateValues" dxfId="5" priority="3685"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3685"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="duplicateValues" dxfId="4" priority="3684"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3684"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A23:A1048576 A1:A5">
-    <cfRule type="duplicateValues" dxfId="3" priority="3683"/>
+  <conditionalFormatting sqref="A22:A1048576 A1:A5">
+    <cfRule type="duplicateValues" dxfId="1" priority="3683"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6:A22">
-    <cfRule type="duplicateValues" dxfId="2" priority="3721"/>
+  <conditionalFormatting sqref="A6:A21">
+    <cfRule type="duplicateValues" dxfId="0" priority="3951"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:I11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="32.25">
-      <c r="A1" s="42" t="s">
-        <v>287</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75">
-      <c r="A2" s="43" t="s">
-        <v>288</v>
-      </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="44"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="28" t="s">
-        <v>289</v>
-      </c>
-      <c r="B4" s="29">
-        <f ca="1">TODAY()</f>
-        <v>44028</v>
-      </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-    </row>
-    <row r="5" spans="1:9" ht="54">
-      <c r="A5" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>286</v>
-      </c>
-      <c r="D5" s="38" t="s">
-        <v>277</v>
-      </c>
-      <c r="E5" s="38" t="s">
-        <v>129</v>
-      </c>
-      <c r="F5" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="G5" s="39" t="s">
-        <v>131</v>
-      </c>
-      <c r="H5" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="I5" s="40" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="60" customHeight="1">
-      <c r="A6" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="32">
-        <v>1300000</v>
-      </c>
-      <c r="D6" s="33">
-        <v>678155</v>
-      </c>
-      <c r="E6" s="41">
-        <v>0.52</v>
-      </c>
-      <c r="F6" s="34">
-        <v>0</v>
-      </c>
-      <c r="G6" s="35">
-        <v>0</v>
-      </c>
-      <c r="H6" s="30">
-        <v>0</v>
-      </c>
-      <c r="I6" s="21"/>
-    </row>
-    <row r="7" spans="1:9" ht="60" customHeight="1">
-      <c r="A7" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="32">
-        <v>1000000</v>
-      </c>
-      <c r="D7" s="33">
-        <v>623245</v>
-      </c>
-      <c r="E7" s="41">
-        <v>0.62</v>
-      </c>
-      <c r="F7" s="34">
-        <v>0</v>
-      </c>
-      <c r="G7" s="35">
-        <v>0</v>
-      </c>
-      <c r="H7" s="30">
-        <v>0</v>
-      </c>
-      <c r="I7" s="21"/>
-    </row>
-    <row r="8" spans="1:9" ht="60" customHeight="1">
-      <c r="A8" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" s="32">
-        <v>900000</v>
-      </c>
-      <c r="D8" s="33">
-        <v>556360</v>
-      </c>
-      <c r="E8" s="41">
-        <v>0.62</v>
-      </c>
-      <c r="F8" s="34">
-        <v>0</v>
-      </c>
-      <c r="G8" s="35">
-        <v>0</v>
-      </c>
-      <c r="H8" s="30">
-        <v>0</v>
-      </c>
-      <c r="I8" s="21"/>
-    </row>
-    <row r="9" spans="1:9" ht="60" customHeight="1">
-      <c r="A9" s="31" t="s">
-        <v>241</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>242</v>
-      </c>
-      <c r="C9" s="32">
-        <v>800000</v>
-      </c>
-      <c r="D9" s="33">
-        <v>438740</v>
-      </c>
-      <c r="E9" s="41">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="F9" s="34">
-        <v>0</v>
-      </c>
-      <c r="G9" s="35">
-        <v>90</v>
-      </c>
-      <c r="H9" s="30">
-        <v>90</v>
-      </c>
-      <c r="I9" s="21"/>
-    </row>
-    <row r="10" spans="1:9" ht="60" customHeight="1">
-      <c r="A10" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="B10" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="32">
-        <v>381157</v>
-      </c>
-      <c r="D10" s="33">
-        <v>251605</v>
-      </c>
-      <c r="E10" s="41">
-        <v>0.66</v>
-      </c>
-      <c r="F10" s="34">
-        <v>0</v>
-      </c>
-      <c r="G10" s="35">
-        <v>0</v>
-      </c>
-      <c r="H10" s="30">
-        <v>0</v>
-      </c>
-      <c r="I10" s="21"/>
-    </row>
-    <row r="11" spans="1:9" ht="60" customHeight="1">
-      <c r="A11" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="32">
-        <v>350000</v>
-      </c>
-      <c r="D11" s="33">
-        <v>291550</v>
-      </c>
-      <c r="E11" s="41">
-        <v>0.83</v>
-      </c>
-      <c r="F11" s="34">
-        <v>1453</v>
-      </c>
-      <c r="G11" s="35">
-        <v>0</v>
-      </c>
-      <c r="H11" s="30">
-        <v>1453</v>
-      </c>
-      <c r="I11" s="21"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
-  </mergeCells>
-  <conditionalFormatting sqref="A5">
-    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A6:A11">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0" right="0" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="68" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>